<commit_message>
--Split functions into separate files and modules
</commit_message>
<xml_diff>
--- a/pitch_testing_data.xlsx
+++ b/pitch_testing_data.xlsx
@@ -8,20 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>150 cm between bot + person</t>
-  </si>
-  <si>
-    <t>dist btwn obj + person (cm)</t>
   </si>
   <si>
     <t>100 cm between bot + person</t>
@@ -32,12 +27,27 @@
   <si>
     <t>experimental angle (deg)</t>
   </si>
+  <si>
+    <t>adjusted angle (deg)</t>
+  </si>
+  <si>
+    <t>avg error (adj. a. and ex. a.)</t>
+  </si>
+  <si>
+    <t>90 deg error (adj. a. and ex. a.)</t>
+  </si>
+  <si>
+    <t>adjusted by avg experimental (deg)</t>
+  </si>
+  <si>
+    <t>adjusted by 90 experimental (deg)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -49,6 +59,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,12 +90,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -119,7 +137,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$8</c:f>
+              <c:f>Sheet1!$A$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -128,30 +146,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$11:$H$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$8:$D$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>35</c:v>
                 </c:pt>
@@ -160,6 +160,18 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -171,7 +183,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$9</c:f>
+              <c:f>Sheet1!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -180,38 +192,170 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$7:$D$7</c:f>
+              <c:f>Sheet1!$B$13:$H$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>49</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
+                <c:pt idx="6">
+                  <c:v>82</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adjusted angle (deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$9:$D$9</c:f>
+              <c:f>Sheet1!$B$12:$H$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adjusted by avg experimental (deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$16:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>49</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adjusted by 90 experimental (deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$17:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
+                </c:pt>
                 <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>61</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>65</c:v>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -249,6 +393,7 @@
         <c:axId val="66339392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -304,7 +449,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3</c:f>
+              <c:f>Sheet1!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -313,36 +458,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$J$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>120</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>150</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$3:$F$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>36</c:v>
                 </c:pt>
@@ -357,6 +478,18 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>73</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -377,50 +510,194 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
-          <c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$F$2</c:f>
+              <c:f>Sheet1!$B$4:$J$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>60</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>80</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150</c:v>
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adjusted angle (deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$F$4</c:f>
+              <c:f>Sheet1!$B$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>57</c:v>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adjusted by avg experimental (deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>60</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>75</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adjusted by 90 experimental (deg)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>62</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>71</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65</c:v>
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -458,6 +735,7 @@
         <c:axId val="520850816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="30"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -492,16 +770,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1504951</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>1743074</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -522,16 +800,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>514349</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>57151</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>1504951</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1800224</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -840,10 +1118,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z10"/>
+  <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,47 +1136,71 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C2">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="E2">
-        <v>120</v>
+        <v>55</v>
       </c>
       <c r="F2">
-        <v>150</v>
+        <v>57</v>
+      </c>
+      <c r="G2">
+        <v>66</v>
+      </c>
+      <c r="H2">
+        <v>69</v>
+      </c>
+      <c r="I2" s="3">
+        <v>76</v>
+      </c>
+      <c r="J2" s="3">
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3">
         <v>45</v>
       </c>
       <c r="D3">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="E3">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F3">
-        <v>57</v>
+        <v>62</v>
+      </c>
+      <c r="G3">
+        <v>67</v>
+      </c>
+      <c r="H3">
+        <v>71</v>
+      </c>
+      <c r="I3" s="3">
+        <v>75</v>
+      </c>
+      <c r="J3" s="3">
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>57</v>
@@ -915,141 +1217,463 @@
       <c r="F4">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
+      <c r="G4">
+        <v>74</v>
+      </c>
+      <c r="H4">
+        <v>83</v>
+      </c>
+      <c r="I4">
+        <v>79</v>
+      </c>
+      <c r="J4">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <f>(SUM(B4:J4) - SUM(B3:J3)) / COUNT(B3:Z3)</f>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="C5">
+        <f>B5</f>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:J5" si="0">C5</f>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>10.777777777777779</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>10.777777777777779</v>
+      </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>J4-J3</f>
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <f>B6</f>
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <f>C6</f>
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <f>D6</f>
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <f>E6</f>
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G6:J6" si="1">F6</f>
+        <v>10</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B7">
+        <f>ROUND(B4 - B5, 0)</f>
+        <v>46</v>
+      </c>
+      <c r="C7">
+        <f t="shared" ref="C7:J7" si="2">ROUND(C4 - C5, 0)</f>
+        <v>49</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
-      <c r="C7">
-        <v>80</v>
-      </c>
-      <c r="D7">
-        <v>100</v>
+      <c r="F7">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>63</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>72</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="2"/>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <f>B4-B6</f>
+        <v>47</v>
+      </c>
+      <c r="C8">
+        <f t="shared" ref="C8:J8" si="3">C4-C6</f>
+        <v>50</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="3"/>
+        <v>52</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>61</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="3"/>
+        <v>55</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>73</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="2"/>
+      <c r="S9" s="2"/>
+      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
+      <c r="V9" s="2"/>
+      <c r="W9" s="2"/>
+      <c r="X9" s="2"/>
+      <c r="Y9" s="2"/>
+      <c r="Z9" s="2"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11">
+        <v>35</v>
+      </c>
+      <c r="C11">
+        <v>44</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
+      </c>
+      <c r="E11">
+        <v>54</v>
+      </c>
+      <c r="F11">
+        <v>59</v>
+      </c>
+      <c r="G11" s="4">
+        <v>62</v>
+      </c>
+      <c r="H11" s="4">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>37</v>
+      </c>
+      <c r="C12">
+        <v>45</v>
+      </c>
+      <c r="D12">
+        <v>51</v>
+      </c>
+      <c r="E12">
+        <v>57</v>
+      </c>
+      <c r="F12">
+        <v>63</v>
+      </c>
+      <c r="G12" s="4">
+        <v>69</v>
+      </c>
+      <c r="H12" s="4">
+        <v>70</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
-        <v>35</v>
-      </c>
-      <c r="C8">
-        <v>44</v>
-      </c>
-      <c r="D8">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9">
+      <c r="B13">
         <v>49</v>
       </c>
-      <c r="C9">
+      <c r="C13">
         <v>61</v>
       </c>
-      <c r="D9">
+      <c r="D13">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="126.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
+      <c r="E13">
+        <v>66</v>
+      </c>
+      <c r="F13">
+        <v>73</v>
+      </c>
+      <c r="G13">
+        <v>80</v>
+      </c>
+      <c r="H13">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <f>(SUM(B13:J13) - SUM(B12:J12)) / COUNT(B12:Z12)</f>
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <f>B14</f>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:H14" si="4">C14</f>
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15">
+        <f>H13-H12</f>
+        <v>12</v>
+      </c>
+      <c r="C15">
+        <f>B15</f>
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ref="D15:H15" si="5">C15</f>
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16">
+        <f>ROUND(B13 - B14, 0)</f>
+        <v>37</v>
+      </c>
+      <c r="C16">
+        <f t="shared" ref="C16:H16" si="6">ROUND(C13 - C14, 0)</f>
+        <v>49</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="6"/>
+        <v>53</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="6"/>
+        <v>54</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="6"/>
+        <v>61</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="6"/>
+        <v>68</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17">
+        <f>B13-B15</f>
+        <v>37</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:H17" si="7">C13-C15</f>
+        <v>49</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="7"/>
+        <v>53</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="7"/>
+        <v>54</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="7"/>
+        <v>61</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="7"/>
+        <v>68</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" ht="141" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2"/>
+      <c r="T18" s="2"/>
+      <c r="U18" s="2"/>
+      <c r="V18" s="2"/>
+      <c r="W18" s="2"/>
+      <c r="X18" s="2"/>
+      <c r="Y18" s="2"/>
+      <c r="Z18" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A5:Z5"/>
-    <mergeCell ref="A10:Z10"/>
+    <mergeCell ref="A9:Z9"/>
+    <mergeCell ref="A18:Z18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>